<commit_message>
Add other computations to arianna spreadsheet
</commit_message>
<xml_diff>
--- a/comparison_plots/data/arianna_veff_to_aff_calculation.xlsx
+++ b/comparison_plots/data/arianna_veff_to_aff_calculation.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="991" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="982" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t>Log10(E/eV)</t>
   </si>
@@ -31,7 +31,7 @@
     <t>Vomega_eff(km^3 sr)</t>
   </si>
   <si>
-    <t>Vomega_eff(cm^2 sr)</t>
+    <t>Vomega_eff(cm^3 sr)</t>
   </si>
   <si>
     <t>sigma(cm^2)</t>
@@ -41,6 +41,15 @@
   </si>
   <si>
     <t>Aomega_eff(cm^2 sr)</t>
+  </si>
+  <si>
+    <t>aomega_eff(km^2 sr)</t>
+  </si>
+  <si>
+    <t>lint(cm)</t>
+  </si>
+  <si>
+    <t>lin(km)</t>
   </si>
 </sst>
 </file>
@@ -147,18 +156,16 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:G13"/>
+  <dimension ref="A1:G30"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D2" activeCellId="0" sqref="D2"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A7" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C31" activeCellId="0" sqref="C31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="2" min="1" style="0" width="11.3418367346939"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="20.3826530612245"/>
-    <col collapsed="false" hidden="false" max="5" min="4" style="0" width="15.9285714285714"/>
-    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="11.3418367346939"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="20.1122448979592"/>
+    <col collapsed="false" hidden="false" max="5" min="4" style="0" width="15.6581632653061"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -518,6 +525,217 @@
       <c r="G13" s="0" t="n">
         <f aca="false">D13/F13</f>
         <v>4022899946.09642</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B20" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="C20" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="D20" s="0" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="0" t="n">
+        <v>-6.424895917</v>
+      </c>
+      <c r="B21" s="0" t="n">
+        <f aca="false">10^A21</f>
+        <v>3.75927488261644E-007</v>
+      </c>
+      <c r="C21" s="0" t="n">
+        <v>161293479.880792</v>
+      </c>
+      <c r="D21" s="0" t="n">
+        <f aca="false">C21/100000</f>
+        <v>1612.93479880792</v>
+      </c>
+      <c r="E21" s="0" t="n">
+        <f aca="false">D21*B21</f>
+        <v>0.000606346527645661</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="0" t="n">
+        <v>-4.848875917</v>
+      </c>
+      <c r="B22" s="0" t="n">
+        <f aca="false">10^A22</f>
+        <v>1.41619834654874E-005</v>
+      </c>
+      <c r="C22" s="0" t="n">
+        <v>106198115.902776</v>
+      </c>
+      <c r="D22" s="0" t="n">
+        <f aca="false">C22/100000</f>
+        <v>1061.98115902776</v>
+      </c>
+      <c r="E22" s="0" t="n">
+        <f aca="false">D22*B22</f>
+        <v>0.0150397596148103</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="0" t="n">
+        <v>-3.819635917</v>
+      </c>
+      <c r="B23" s="0" t="n">
+        <f aca="false">10^A23</f>
+        <v>0.000151483064741315</v>
+      </c>
+      <c r="C23" s="0" t="n">
+        <v>69922478.1413035</v>
+      </c>
+      <c r="D23" s="0" t="n">
+        <f aca="false">C23/100000</f>
+        <v>699.224781413035</v>
+      </c>
+      <c r="E23" s="0" t="n">
+        <f aca="false">D23*B23</f>
+        <v>0.105920712831523</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="0" t="n">
+        <v>-3.047705917</v>
+      </c>
+      <c r="B24" s="0" t="n">
+        <f aca="false">10^A24</f>
+        <v>0.000895971268137834</v>
+      </c>
+      <c r="C24" s="0" t="n">
+        <v>46038038.5081131</v>
+      </c>
+      <c r="D24" s="0" t="n">
+        <f aca="false">C24/100000</f>
+        <v>460.380385081131</v>
+      </c>
+      <c r="E24" s="0" t="n">
+        <f aca="false">D24*B24</f>
+        <v>0.412487597446925</v>
+      </c>
+    </row>
+    <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="0" t="n">
+        <v>-2.404435917</v>
+      </c>
+      <c r="B25" s="0" t="n">
+        <f aca="false">10^A25</f>
+        <v>0.00394061569724877</v>
+      </c>
+      <c r="C25" s="0" t="n">
+        <v>30312154.9180693</v>
+      </c>
+      <c r="D25" s="0" t="n">
+        <f aca="false">C25/100000</f>
+        <v>303.121549180693</v>
+      </c>
+      <c r="E25" s="0" t="n">
+        <f aca="false">D25*B25</f>
+        <v>1.1944855348758</v>
+      </c>
+    </row>
+    <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="0" t="n">
+        <v>-1.857645917</v>
+      </c>
+      <c r="B26" s="0" t="n">
+        <f aca="false">10^A26</f>
+        <v>0.0138788692057944</v>
+      </c>
+      <c r="C26" s="0" t="n">
+        <v>19957990.512891</v>
+      </c>
+      <c r="D26" s="0" t="n">
+        <f aca="false">C26/100000</f>
+        <v>199.57990512891</v>
+      </c>
+      <c r="E26" s="0" t="n">
+        <f aca="false">D26*B26</f>
+        <v>2.769943399389</v>
+      </c>
+    </row>
+    <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="0" t="n">
+        <v>-1.439515917</v>
+      </c>
+      <c r="B27" s="0" t="n">
+        <f aca="false">10^A27</f>
+        <v>0.0363482982560892</v>
+      </c>
+      <c r="C27" s="0" t="n">
+        <v>13140648.9043511</v>
+      </c>
+      <c r="D27" s="0" t="n">
+        <f aca="false">C27/100000</f>
+        <v>131.406489043511</v>
+      </c>
+      <c r="E27" s="0" t="n">
+        <f aca="false">D27*B27</f>
+        <v>4.77640225653905</v>
+      </c>
+    </row>
+    <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A28" s="0" t="n">
+        <v>-1.021395917</v>
+      </c>
+      <c r="B28" s="0" t="n">
+        <f aca="false">10^A28</f>
+        <v>0.0951927959798031</v>
+      </c>
+      <c r="C28" s="0" t="n">
+        <v>8652005.99809334</v>
+      </c>
+      <c r="D28" s="0" t="n">
+        <f aca="false">C28/100000</f>
+        <v>86.5200599809334</v>
+      </c>
+      <c r="E28" s="0" t="n">
+        <f aca="false">D28*B28</f>
+        <v>8.23608641792533</v>
+      </c>
+    </row>
+    <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A29" s="0" t="n">
+        <v>-0.6997559174</v>
+      </c>
+      <c r="B29" s="0" t="n">
+        <f aca="false">10^A29</f>
+        <v>0.19963840093814</v>
+      </c>
+      <c r="C29" s="0" t="n">
+        <v>5696614.24910735</v>
+      </c>
+      <c r="D29" s="0" t="n">
+        <f aca="false">C29/100000</f>
+        <v>56.9661424910735</v>
+      </c>
+      <c r="E29" s="0" t="n">
+        <f aca="false">D29*B29</f>
+        <v>11.3726295945322</v>
+      </c>
+    </row>
+    <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A30" s="0" t="n">
+        <v>-0.5067759174</v>
+      </c>
+      <c r="B30" s="0" t="n">
+        <f aca="false">10^A30</f>
+        <v>0.311332230134271</v>
+      </c>
+      <c r="C30" s="0" t="n">
+        <v>3750738.72004761</v>
+      </c>
+      <c r="D30" s="0" t="n">
+        <f aca="false">C30/100000</f>
+        <v>37.5073872004761</v>
+      </c>
+      <c r="E30" s="0" t="n">
+        <f aca="false">D30*B30</f>
+        <v>11.6772585036338</v>
       </c>
     </row>
   </sheetData>

</xml_diff>